<commit_message>
RNA test plus bug fixes
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckostiw/C3G/repos/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678D4B5-90BC-F849-A682-CAED5115FBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948C67B5-BEAD-944D-B1FA-575E5D1C588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28700" windowHeight="17320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28720" yWindow="6500" windowWidth="28700" windowHeight="17320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LibraryQC" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="430">
   <si>
     <t>Library QC Template</t>
   </si>
@@ -1347,6 +1347,12 @@
   </si>
   <si>
     <t>comment2</t>
+  </si>
+  <si>
+    <t>LIBRARY_SAMPLE_3</t>
+  </si>
+  <si>
+    <t>comment3</t>
   </si>
 </sst>
 </file>
@@ -2097,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q710"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2285,26 +2291,56 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="A10" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="12">
+        <v>100</v>
+      </c>
+      <c r="E10" s="13">
+        <v>100</v>
+      </c>
+      <c r="F10" s="13">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="13">
+        <v>100</v>
+      </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="13" t="str">
+      <c r="K10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="18"/>
+        <v>2734.011</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q10" s="18" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>

</xml_diff>

<commit_message>
Fixed the version of the templates
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckostiw/C3G/repos/freezeman/backend/fms_core/tests/valid_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948C67B5-BEAD-944D-B1FA-575E5D1C588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00992E5-BF28-9E48-9D6C-6281B64338CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28720" yWindow="6500" windowWidth="28700" windowHeight="17320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,8 @@
     <definedName name="Double_stranded">Index!$H$2</definedName>
     <definedName name="Single_stranded">Index!$I$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -63,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="432">
   <si>
     <t>Library QC Template</t>
   </si>
@@ -1353,13 +1343,19 @@
   </si>
   <si>
     <t>comment3</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>3.9.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1413,6 +1409,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1655,7 +1657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1719,6 +1721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2103,9 +2106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q710"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2134,6 +2135,20 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="O2"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+    </row>
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" s="33"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
LibQC test first iteration
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00992E5-BF28-9E48-9D6C-6281B64338CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3D94D4-BF9D-6C4F-BF28-11F13619B97E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28720" yWindow="6500" windowWidth="28700" windowHeight="17320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37200" yWindow="500" windowWidth="37180" windowHeight="23080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LibraryQC" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="434">
   <si>
     <t>Library QC Template</t>
   </si>
@@ -1349,6 +1349,12 @@
   </si>
   <si>
     <t>3.9.0</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>POOL_LIBRARIES</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1722,6 +1728,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2358,26 +2365,56 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="A11" s="34" t="s">
+        <v>433</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="12">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13">
+        <v>100</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="13">
+        <v>100</v>
+      </c>
       <c r="J11" s="13"/>
-      <c r="K11" s="13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
+      <c r="K11" s="13">
+        <f t="shared" ref="K11" ca="1" si="1">IF(OR(ISBLANK(E11),AND(OR(ISBLANK(G11),ISBLANK(H11),ISBLANK(I11)),ISBLANK(J11))),"",IF(ISBLANK(J11),(E11-F11)*I11*H11*INDIRECT(SUBSTITUTE(G11," ","_"))/1000000,(E11-F11)*J11))</f>
+        <v>2734.011</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
@@ -3007,7 +3044,7 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13" t="str">
-        <f t="shared" ref="K40:K71" ca="1" si="1">IF(OR(ISBLANK(E40),AND(OR(ISBLANK(G40),ISBLANK(H40),ISBLANK(I40)),ISBLANK(J40))),"",IF(ISBLANK(J40),(E40-F40)*I40*H40*INDIRECT(SUBSTITUTE(G40," ","_"))/1000000,(E40-F40)*J40))</f>
+        <f t="shared" ref="K40:K71" ca="1" si="2">IF(OR(ISBLANK(E40),AND(OR(ISBLANK(G40),ISBLANK(H40),ISBLANK(I40)),ISBLANK(J40))),"",IF(ISBLANK(J40),(E40-F40)*I40*H40*INDIRECT(SUBSTITUTE(G40," ","_"))/1000000,(E40-F40)*J40))</f>
         <v/>
       </c>
       <c r="L40" s="15"/>
@@ -3029,7 +3066,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L41" s="15"/>
@@ -3051,7 +3088,7 @@
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L42" s="15"/>
@@ -3073,7 +3110,7 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L43" s="15"/>
@@ -3095,7 +3132,7 @@
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L44" s="15"/>
@@ -3117,7 +3154,7 @@
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
       <c r="K45" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L45" s="15"/>
@@ -3139,7 +3176,7 @@
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
       <c r="K46" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L46" s="15"/>
@@ -3161,7 +3198,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
       <c r="K47" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L47" s="15"/>
@@ -3183,7 +3220,7 @@
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L48" s="15"/>
@@ -3205,7 +3242,7 @@
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L49" s="15"/>
@@ -3227,7 +3264,7 @@
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
       <c r="K50" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L50" s="15"/>
@@ -3249,7 +3286,7 @@
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L51" s="15"/>
@@ -3271,7 +3308,7 @@
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L52" s="15"/>
@@ -3293,7 +3330,7 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L53" s="15"/>
@@ -3315,7 +3352,7 @@
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L54" s="15"/>
@@ -3337,7 +3374,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
       <c r="K55" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L55" s="15"/>
@@ -3359,7 +3396,7 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
       <c r="K56" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L56" s="15"/>
@@ -3381,7 +3418,7 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L57" s="15"/>
@@ -3403,7 +3440,7 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L58" s="15"/>
@@ -3425,7 +3462,7 @@
       <c r="I59" s="13"/>
       <c r="J59" s="13"/>
       <c r="K59" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L59" s="15"/>
@@ -3447,7 +3484,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
       <c r="K60" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L60" s="15"/>
@@ -3469,7 +3506,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L61" s="15"/>
@@ -3491,7 +3528,7 @@
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
       <c r="K62" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L62" s="15"/>
@@ -3513,7 +3550,7 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L63" s="15"/>
@@ -3535,7 +3572,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
       <c r="K64" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L64" s="15"/>
@@ -3557,7 +3594,7 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L65" s="15"/>
@@ -3579,7 +3616,7 @@
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
       <c r="K66" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L66" s="15"/>
@@ -3601,7 +3638,7 @@
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
       <c r="K67" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L67" s="15"/>
@@ -3623,7 +3660,7 @@
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
       <c r="K68" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L68" s="15"/>
@@ -3645,7 +3682,7 @@
       <c r="I69" s="13"/>
       <c r="J69" s="13"/>
       <c r="K69" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L69" s="15"/>
@@ -3667,7 +3704,7 @@
       <c r="I70" s="13"/>
       <c r="J70" s="13"/>
       <c r="K70" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L70" s="15"/>
@@ -3689,7 +3726,7 @@
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
       <c r="K71" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
       <c r="L71" s="15"/>
@@ -3711,7 +3748,7 @@
       <c r="I72" s="13"/>
       <c r="J72" s="13"/>
       <c r="K72" s="13" t="str">
-        <f t="shared" ref="K72:K103" ca="1" si="2">IF(OR(ISBLANK(E72),AND(OR(ISBLANK(G72),ISBLANK(H72),ISBLANK(I72)),ISBLANK(J72))),"",IF(ISBLANK(J72),(E72-F72)*I72*H72*INDIRECT(SUBSTITUTE(G72," ","_"))/1000000,(E72-F72)*J72))</f>
+        <f t="shared" ref="K72:K103" ca="1" si="3">IF(OR(ISBLANK(E72),AND(OR(ISBLANK(G72),ISBLANK(H72),ISBLANK(I72)),ISBLANK(J72))),"",IF(ISBLANK(J72),(E72-F72)*I72*H72*INDIRECT(SUBSTITUTE(G72," ","_"))/1000000,(E72-F72)*J72))</f>
         <v/>
       </c>
       <c r="L72" s="15"/>
@@ -3733,7 +3770,7 @@
       <c r="I73" s="13"/>
       <c r="J73" s="13"/>
       <c r="K73" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L73" s="15"/>
@@ -3755,7 +3792,7 @@
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
       <c r="K74" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L74" s="15"/>
@@ -3777,7 +3814,7 @@
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L75" s="15"/>
@@ -3799,7 +3836,7 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
       <c r="K76" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L76" s="15"/>
@@ -3821,7 +3858,7 @@
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
       <c r="K77" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L77" s="15"/>
@@ -3843,7 +3880,7 @@
       <c r="I78" s="13"/>
       <c r="J78" s="13"/>
       <c r="K78" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L78" s="15"/>
@@ -3865,7 +3902,7 @@
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
       <c r="K79" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L79" s="15"/>
@@ -3887,7 +3924,7 @@
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
       <c r="K80" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L80" s="15"/>
@@ -3909,7 +3946,7 @@
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
       <c r="K81" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L81" s="15"/>
@@ -3931,7 +3968,7 @@
       <c r="I82" s="13"/>
       <c r="J82" s="13"/>
       <c r="K82" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L82" s="15"/>
@@ -3953,7 +3990,7 @@
       <c r="I83" s="13"/>
       <c r="J83" s="13"/>
       <c r="K83" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L83" s="15"/>
@@ -3975,7 +4012,7 @@
       <c r="I84" s="13"/>
       <c r="J84" s="13"/>
       <c r="K84" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L84" s="15"/>
@@ -3997,7 +4034,7 @@
       <c r="I85" s="13"/>
       <c r="J85" s="13"/>
       <c r="K85" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L85" s="15"/>
@@ -4019,7 +4056,7 @@
       <c r="I86" s="13"/>
       <c r="J86" s="13"/>
       <c r="K86" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L86" s="15"/>
@@ -4041,7 +4078,7 @@
       <c r="I87" s="13"/>
       <c r="J87" s="13"/>
       <c r="K87" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L87" s="15"/>
@@ -4063,7 +4100,7 @@
       <c r="I88" s="13"/>
       <c r="J88" s="13"/>
       <c r="K88" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L88" s="15"/>
@@ -4085,7 +4122,7 @@
       <c r="I89" s="13"/>
       <c r="J89" s="13"/>
       <c r="K89" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L89" s="15"/>
@@ -4107,7 +4144,7 @@
       <c r="I90" s="13"/>
       <c r="J90" s="13"/>
       <c r="K90" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L90" s="15"/>
@@ -4129,7 +4166,7 @@
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L91" s="15"/>
@@ -4151,7 +4188,7 @@
       <c r="I92" s="13"/>
       <c r="J92" s="13"/>
       <c r="K92" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L92" s="15"/>
@@ -4173,7 +4210,7 @@
       <c r="I93" s="13"/>
       <c r="J93" s="13"/>
       <c r="K93" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L93" s="15"/>
@@ -4195,7 +4232,7 @@
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L94" s="15"/>
@@ -4217,7 +4254,7 @@
       <c r="I95" s="13"/>
       <c r="J95" s="13"/>
       <c r="K95" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L95" s="15"/>
@@ -4239,7 +4276,7 @@
       <c r="I96" s="13"/>
       <c r="J96" s="13"/>
       <c r="K96" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L96" s="15"/>
@@ -4261,7 +4298,7 @@
       <c r="I97" s="13"/>
       <c r="J97" s="13"/>
       <c r="K97" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L97" s="15"/>
@@ -4283,7 +4320,7 @@
       <c r="I98" s="13"/>
       <c r="J98" s="13"/>
       <c r="K98" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L98" s="15"/>
@@ -4305,7 +4342,7 @@
       <c r="I99" s="13"/>
       <c r="J99" s="13"/>
       <c r="K99" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L99" s="15"/>
@@ -4327,7 +4364,7 @@
       <c r="I100" s="13"/>
       <c r="J100" s="13"/>
       <c r="K100" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L100" s="15"/>
@@ -4349,7 +4386,7 @@
       <c r="I101" s="13"/>
       <c r="J101" s="13"/>
       <c r="K101" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L101" s="15"/>
@@ -4371,7 +4408,7 @@
       <c r="I102" s="13"/>
       <c r="J102" s="13"/>
       <c r="K102" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L102" s="15"/>
@@ -4393,7 +4430,7 @@
       <c r="I103" s="24"/>
       <c r="J103" s="24"/>
       <c r="K103" s="24" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="L103" s="26"/>

</xml_diff>

<commit_message>
Fixed normalization test due to lack of concentration and added LibraryQCtest
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_QC_v3_9_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3D94D4-BF9D-6C4F-BF28-11F13619B97E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5BC0DA-3AD0-1146-991E-9B291DEFD76D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="500" windowWidth="37180" windowHeight="23080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LibraryQC" sheetId="1" r:id="rId1"/>
@@ -2113,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q710"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>